<commit_message>
Dynamic Fitur Hasil Nilai Ujian Siswa
</commit_message>
<xml_diff>
--- a/data/XII-MIA-1.xlsx
+++ b/data/XII-MIA-1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tugas Akhir\Development\New Develop\Aplikasi-Penilaian-Otomatis-Esai-BI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="SOAL-1-XII-MIA-1" sheetId="2" r:id="rId1"/>
-    <sheet name="SOAL-2-XII-MIA-2" sheetId="1" r:id="rId2"/>
+    <sheet name="SOAL-2-XII-MIA-1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -627,9 +627,6 @@
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -709,6 +706,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -995,986 +995,987 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="130" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="130" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="31" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="31" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+      <c r="A8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="14">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="13">
         <v>1</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="32" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="31" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="18">
-        <v>40</v>
-      </c>
-      <c r="E14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="17">
+        <v>50</v>
+      </c>
+      <c r="E14" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>1</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="34">
-        <v>30</v>
+      <c r="E17" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>2</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D18" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="34">
-        <v>40</v>
+      <c r="E18" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
+      <c r="A19" s="19">
         <v>3</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>26</v>
       </c>
       <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="34">
-        <v>40</v>
+      <c r="E19" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="19">
         <v>4</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="34">
-        <v>40</v>
+      <c r="E20" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="19">
         <v>5</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D21" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="34">
-        <v>40</v>
+      <c r="E21" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="19">
         <v>6</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>35</v>
       </c>
       <c r="D22" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="34">
-        <v>30</v>
+      <c r="E22" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="19">
         <v>7</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
         <v>107</v>
       </c>
-      <c r="E23" s="34">
+      <c r="E23" s="33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>8</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>8</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D24" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="34">
-        <v>10</v>
+      <c r="E24" s="33">
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
+      <c r="A25" s="19">
         <v>9</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="34">
-        <v>20</v>
+      <c r="E25" s="33">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="A26" s="19">
         <v>10</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>47</v>
       </c>
       <c r="D26" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="34">
-        <v>30</v>
+      <c r="E26" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
+      <c r="A27" s="19">
         <v>11</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="34">
-        <v>30</v>
+      <c r="E27" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+      <c r="A28" s="19">
         <v>12</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>53</v>
       </c>
       <c r="D28" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="34">
-        <v>25</v>
+      <c r="E28" s="33">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
+      <c r="A29" s="19">
         <v>13</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="26" t="s">
         <v>56</v>
       </c>
       <c r="D29" t="s">
         <v>113</v>
       </c>
-      <c r="E29" s="34">
-        <v>40</v>
+      <c r="E29" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
+      <c r="A30" s="19">
         <v>14</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>59</v>
       </c>
       <c r="D30" t="s">
         <v>114</v>
       </c>
-      <c r="E30" s="34">
-        <v>40</v>
+      <c r="E30" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
+      <c r="A31" s="19">
         <v>15</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>62</v>
       </c>
       <c r="D31" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="34">
-        <v>40</v>
+      <c r="E31" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
+      <c r="A32" s="19">
         <v>16</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>65</v>
       </c>
       <c r="D32" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="34">
-        <v>40</v>
+      <c r="E32" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="A33" s="19">
         <v>17</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>68</v>
       </c>
       <c r="D33" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="34">
-        <v>30</v>
+      <c r="E33" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
+      <c r="A34" s="19">
         <v>18</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D34" t="s">
         <v>113</v>
       </c>
-      <c r="E34" s="34">
-        <v>30</v>
+      <c r="E34" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
+      <c r="A35" s="19">
         <v>19</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="21" t="s">
         <v>73</v>
       </c>
       <c r="D35" t="s">
         <v>118</v>
       </c>
-      <c r="E35" s="34">
-        <v>40</v>
+      <c r="E35" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
+      <c r="A36" s="19">
         <v>20</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>76</v>
       </c>
       <c r="D36" t="s">
         <v>119</v>
       </c>
-      <c r="E36" s="34">
-        <v>10</v>
+      <c r="E36" s="33">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
+      <c r="A37" s="19">
         <v>21</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D37" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="34">
-        <v>30</v>
+      <c r="E37" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
+      <c r="A38" s="19">
         <v>22</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="21" t="s">
         <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="34">
-        <v>30</v>
+      <c r="E38" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="20">
+      <c r="A39" s="19">
         <v>23</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C39" s="21" t="s">
         <v>85</v>
       </c>
       <c r="D39" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="34">
-        <v>40</v>
+      <c r="E39" s="33">
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
+      <c r="A40" s="19">
         <v>24</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>88</v>
       </c>
       <c r="D40" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="34">
-        <v>30</v>
+      <c r="E40" s="33">
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
+      <c r="A41" s="19">
         <v>25</v>
       </c>
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="26" t="s">
         <v>91</v>
       </c>
       <c r="D41" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="34">
-        <v>15</v>
+      <c r="E41" s="33">
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
+      <c r="A42" s="19">
         <v>26</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="25"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="20">
+      <c r="A43" s="19">
         <v>27</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="20">
+      <c r="A44" s="19">
         <v>28</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="20">
+      <c r="A45" s="19">
         <v>29</v>
       </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="25"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="20">
+      <c r="A46" s="19">
         <v>30</v>
       </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20">
+      <c r="A47" s="19">
         <v>31</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="25"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="20">
+      <c r="A48" s="19">
         <v>32</v>
       </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="20">
+      <c r="A49" s="19">
         <v>33</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="25"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="20">
+      <c r="A50" s="19">
         <v>34</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D51" s="35"/>
-      <c r="E51" s="36"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="35"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D52" s="35"/>
-      <c r="E52" s="36"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="35"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D53" s="35"/>
-      <c r="E53" s="36"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="35"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D54" s="35"/>
-      <c r="E54" s="36"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D55" s="35"/>
-      <c r="E55" s="36"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="35"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D56" s="35"/>
-      <c r="E56" s="36"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="35"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D57" s="35"/>
-      <c r="E57" s="36"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="35"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D58" s="35"/>
-      <c r="E58" s="36"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="35"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D59" s="35"/>
-      <c r="E59" s="36"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="35"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D60" s="35"/>
-      <c r="E60" s="36"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="35"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D61" s="35"/>
-      <c r="E61" s="36"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D62" s="35"/>
-      <c r="E62" s="36"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="35"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D63" s="35"/>
-      <c r="E63" s="36"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="35"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D64" s="35"/>
-      <c r="E64" s="36"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="35"/>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D65" s="35"/>
-      <c r="E65" s="36"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="35"/>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D66" s="35"/>
-      <c r="E66" s="36"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="35"/>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D67" s="35"/>
-      <c r="E67" s="36"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="35"/>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D68" s="35"/>
-      <c r="E68" s="36"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="35"/>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D69" s="35"/>
-      <c r="E69" s="36"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="35"/>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="35"/>
-      <c r="E70" s="36"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="35"/>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D71" s="35"/>
-      <c r="E71" s="36"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="35"/>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D72" s="35"/>
-      <c r="E72" s="36"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="35"/>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D73" s="35"/>
-      <c r="E73" s="36"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="35"/>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D74" s="35"/>
-      <c r="E74" s="36"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="35"/>
     </row>
     <row r="75" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D75" s="35"/>
-      <c r="E75" s="36"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="35"/>
     </row>
     <row r="76" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D76" s="35"/>
-      <c r="E76" s="36"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="35"/>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D77" s="35"/>
-      <c r="E77" s="36"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="35"/>
     </row>
     <row r="78" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D78" s="35"/>
-      <c r="E78" s="36"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="35"/>
     </row>
     <row r="79" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D79" s="35"/>
-      <c r="E79" s="36"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="35"/>
     </row>
     <row r="80" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D80" s="35"/>
-      <c r="E80" s="36"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="35"/>
     </row>
     <row r="81" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D81" s="35"/>
-      <c r="E81" s="36"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="35"/>
     </row>
     <row r="82" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D82" s="35"/>
-      <c r="E82" s="36"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="35"/>
     </row>
     <row r="83" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D83" s="35"/>
-      <c r="E83" s="36"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="35"/>
     </row>
     <row r="84" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D84" s="35"/>
-      <c r="E84" s="36"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="35"/>
     </row>
     <row r="85" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D85" s="35"/>
-      <c r="E85" s="36"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="35"/>
     </row>
     <row r="86" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D86" s="35"/>
-      <c r="E86" s="36"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="35"/>
     </row>
     <row r="87" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D87" s="35"/>
-      <c r="E87" s="36"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="35"/>
     </row>
     <row r="88" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D88" s="35"/>
-      <c r="E88" s="36"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="35"/>
     </row>
     <row r="89" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D89" s="35"/>
-      <c r="E89" s="36"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="35"/>
     </row>
     <row r="90" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D90" s="35"/>
-      <c r="E90" s="36"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="35"/>
     </row>
     <row r="91" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D91" s="35"/>
-      <c r="E91" s="36"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="35"/>
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D92" s="35"/>
-      <c r="E92" s="36"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="35"/>
     </row>
     <row r="93" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="35"/>
-      <c r="E93" s="36"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="35"/>
     </row>
     <row r="94" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D94" s="35"/>
-      <c r="E94" s="36"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="35"/>
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D95" s="35"/>
-      <c r="E95" s="36"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="35"/>
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D96" s="35"/>
-      <c r="E96" s="36"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="35"/>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D97" s="35"/>
-      <c r="E97" s="36"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="35"/>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D98" s="35"/>
-      <c r="E98" s="36"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="35"/>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D99" s="35"/>
-      <c r="E99" s="36"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="35"/>
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D100" s="35"/>
-      <c r="E100" s="36"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="35"/>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D101" s="35"/>
-      <c r="E101" s="36"/>
+      <c r="D101" s="34"/>
+      <c r="E101" s="35"/>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D102" s="35"/>
-      <c r="E102" s="36"/>
+      <c r="D102" s="34"/>
+      <c r="E102" s="35"/>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="35"/>
-      <c r="E103" s="36"/>
+      <c r="D103" s="34"/>
+      <c r="E103" s="35"/>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D104" s="35"/>
-      <c r="E104" s="36"/>
+      <c r="D104" s="34"/>
+      <c r="E104" s="35"/>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D105" s="35"/>
-      <c r="E105" s="36"/>
+      <c r="D105" s="34"/>
+      <c r="E105" s="35"/>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D106" s="35"/>
-      <c r="E106" s="36"/>
+      <c r="D106" s="34"/>
+      <c r="E106" s="35"/>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D107" s="35"/>
-      <c r="E107" s="36"/>
+      <c r="D107" s="34"/>
+      <c r="E107" s="35"/>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D108" s="35"/>
-      <c r="E108" s="36"/>
+      <c r="D108" s="34"/>
+      <c r="E108" s="35"/>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D109" s="35"/>
-      <c r="E109" s="36"/>
+      <c r="D109" s="34"/>
+      <c r="E109" s="35"/>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D110" s="35"/>
-      <c r="E110" s="36"/>
+      <c r="D110" s="34"/>
+      <c r="E110" s="35"/>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D111" s="35"/>
-      <c r="E111" s="36"/>
+      <c r="D111" s="34"/>
+      <c r="E111" s="35"/>
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D112" s="35"/>
-      <c r="E112" s="36"/>
+      <c r="D112" s="34"/>
+      <c r="E112" s="35"/>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D113" s="35"/>
-      <c r="E113" s="36"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="35"/>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D114" s="35"/>
-      <c r="E114" s="36"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="35"/>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D115" s="35"/>
-      <c r="E115" s="36"/>
+      <c r="D115" s="34"/>
+      <c r="E115" s="35"/>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D116" s="35"/>
-      <c r="E116" s="36"/>
+      <c r="D116" s="34"/>
+      <c r="E116" s="35"/>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D117" s="35"/>
-      <c r="E117" s="36"/>
+      <c r="D117" s="34"/>
+      <c r="E117" s="35"/>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D118" s="35"/>
-      <c r="E118" s="36"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="35"/>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D119" s="35"/>
-      <c r="E119" s="36"/>
+      <c r="D119" s="34"/>
+      <c r="E119" s="35"/>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D120" s="35"/>
-      <c r="E120" s="36"/>
+      <c r="D120" s="34"/>
+      <c r="E120" s="35"/>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D121" s="35"/>
-      <c r="E121" s="36"/>
+      <c r="D121" s="34"/>
+      <c r="E121" s="35"/>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D122" s="35"/>
-      <c r="E122" s="36"/>
+      <c r="D122" s="34"/>
+      <c r="E122" s="35"/>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D123" s="35"/>
-      <c r="E123" s="36"/>
+      <c r="D123" s="34"/>
+      <c r="E123" s="35"/>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D124" s="35"/>
-      <c r="E124" s="36"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="35"/>
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D125" s="35"/>
-      <c r="E125" s="36"/>
+      <c r="D125" s="34"/>
+      <c r="E125" s="35"/>
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D126" s="35"/>
-      <c r="E126" s="36"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="35"/>
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D127" s="35"/>
-      <c r="E127" s="36"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1982,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,675 +1996,675 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="14">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="13">
         <v>2</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="18">
-        <v>40</v>
-      </c>
-      <c r="E14" s="12"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="17">
+        <v>50</v>
+      </c>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="19">
         <v>1</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>2</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="20">
-        <v>2</v>
-      </c>
-      <c r="B18" s="21" t="s">
+      <c r="C19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>4</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>5</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>6</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>7</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>8</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>9</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>10</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>11</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>12</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
+        <v>13</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
+        <v>14</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
+        <v>15</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="19">
+        <v>16</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19">
+        <v>17</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="19">
+        <v>18</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="19">
+        <v>19</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="19">
+        <v>20</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="19">
+        <v>21</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="19">
         <v>22</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="B38" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="19">
         <v>23</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="B39" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="19">
         <v>24</v>
       </c>
-      <c r="E18" s="25">
+      <c r="B40" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="19">
+        <v>25</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="24">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="20">
-        <v>3</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="22" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="19">
         <v>26</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="B42" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="24"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="19">
         <v>27</v>
       </c>
-      <c r="E19" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>4</v>
-      </c>
-      <c r="B20" s="21" t="s">
+      <c r="B43" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="24"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="19">
         <v>28</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="24"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="19">
         <v>29</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="19">
         <v>30</v>
       </c>
-      <c r="E20" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>5</v>
-      </c>
-      <c r="B21" s="26" t="s">
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="19">
         <v>31</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="19">
         <v>32</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="19">
         <v>33</v>
       </c>
-      <c r="E21" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
-        <v>6</v>
-      </c>
-      <c r="B22" s="26" t="s">
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="19">
         <v>34</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
-        <v>7</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="20">
-        <v>8</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="20">
-        <v>9</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
-        <v>10</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
-        <v>11</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
-        <v>12</v>
-      </c>
-      <c r="B28" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="20">
-        <v>13</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="20">
-        <v>14</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="20">
-        <v>15</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
-        <v>16</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
-        <v>17</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="20">
-        <v>18</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
-        <v>19</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="20">
-        <v>20</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="100.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20">
-        <v>21</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20">
-        <v>22</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="25">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="20">
-        <v>23</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" s="25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="20">
-        <v>24</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
-        <v>25</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
-        <v>26</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="25"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20">
-        <v>27</v>
-      </c>
-      <c r="B43" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="20">
-        <v>28</v>
-      </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20">
-        <v>29</v>
-      </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="25"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
-        <v>30</v>
-      </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
-        <v>31</v>
-      </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="25"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
-        <v>32</v>
-      </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="20">
-        <v>33</v>
-      </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="25"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
-        <v>34</v>
-      </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Penilaian Manual Web, dan Integrasi Celery
</commit_message>
<xml_diff>
--- a/data/XII-MIA-1.xlsx
+++ b/data/XII-MIA-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tugas Akhir\Development\New Develop\Aplikasi-Penilaian-Otomatis-Esai-BI\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyek TA\Aplikasi-Penilaian-Otomatis-Esai-BI\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20FFA15-C66B-4ACF-994F-04C91EDC7348}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6E3415-5F10-4111-A335-75300349D975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOAL-1-XII-MIA-1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="123">
   <si>
     <t>TEMPLATE PENILAIAN MANUAL</t>
   </si>
@@ -401,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +467,18 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -488,7 +500,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -604,6 +616,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -611,7 +636,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -656,15 +681,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -688,9 +704,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -991,13 +1044,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1005,7 +1058,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="24" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="4"/>
@@ -1047,7 +1100,7 @@
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="24" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="11"/>
@@ -1072,7 +1125,7 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="25" t="s">
         <v>97</v>
       </c>
       <c r="E10" s="7"/>
@@ -1083,7 +1136,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="28"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -1092,7 +1145,7 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="24" t="s">
         <v>98</v>
       </c>
       <c r="E12" s="7"/>
@@ -1131,7 +1184,7 @@
       <c r="E16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
@@ -1143,10 +1196,10 @@
       <c r="C17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1160,10 +1213,10 @@
       <c r="C18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1177,10 +1230,10 @@
       <c r="C19" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1194,10 +1247,10 @@
       <c r="C20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1205,16 +1258,16 @@
       <c r="A21" s="19">
         <v>5</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E21" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1222,16 +1275,16 @@
       <c r="A22" s="19">
         <v>6</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1239,16 +1292,16 @@
       <c r="A23" s="19">
         <v>7</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1256,16 +1309,16 @@
       <c r="A24" s="19">
         <v>8</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="22" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="27">
         <v>20</v>
       </c>
     </row>
@@ -1273,16 +1326,16 @@
       <c r="A25" s="19">
         <v>9</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="27">
         <v>30</v>
       </c>
     </row>
@@ -1290,16 +1343,16 @@
       <c r="A26" s="19">
         <v>10</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1307,16 +1360,16 @@
       <c r="A27" s="19">
         <v>11</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1324,16 +1377,16 @@
       <c r="A28" s="19">
         <v>12</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="22" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="27">
         <v>35</v>
       </c>
     </row>
@@ -1341,16 +1394,16 @@
       <c r="A29" s="19">
         <v>13</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1358,16 +1411,16 @@
       <c r="A30" s="19">
         <v>14</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="E30" s="30">
+      <c r="E30" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1375,16 +1428,16 @@
       <c r="A31" s="19">
         <v>15</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="22" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1392,16 +1445,16 @@
       <c r="A32" s="19">
         <v>16</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1409,16 +1462,16 @@
       <c r="A33" s="19">
         <v>17</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1426,16 +1479,16 @@
       <c r="A34" s="19">
         <v>18</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1443,16 +1496,16 @@
       <c r="A35" s="19">
         <v>19</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="22" t="s">
         <v>72</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1460,16 +1513,16 @@
       <c r="A36" s="19">
         <v>20</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="22" t="s">
         <v>75</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="27">
         <v>20</v>
       </c>
     </row>
@@ -1477,16 +1530,16 @@
       <c r="A37" s="19">
         <v>21</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1494,16 +1547,16 @@
       <c r="A38" s="19">
         <v>22</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="22" t="s">
         <v>81</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1511,16 +1564,16 @@
       <c r="A39" s="19">
         <v>23</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="22" t="s">
         <v>84</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="E39" s="30">
+      <c r="E39" s="27">
         <v>50</v>
       </c>
     </row>
@@ -1528,16 +1581,16 @@
       <c r="A40" s="19">
         <v>24</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="22" t="s">
         <v>87</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="27">
         <v>40</v>
       </c>
     </row>
@@ -1548,319 +1601,319 @@
       <c r="B41" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="27">
         <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D42" s="31"/>
-      <c r="E42" s="32"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="29"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="29"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D44" s="31"/>
-      <c r="E44" s="32"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D45" s="31"/>
-      <c r="E45" s="32"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D46" s="31"/>
-      <c r="E46" s="32"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D47" s="31"/>
-      <c r="E47" s="32"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D48" s="31"/>
-      <c r="E48" s="32"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29"/>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="29"/>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D50" s="31"/>
-      <c r="E50" s="32"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="29"/>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D51" s="31"/>
-      <c r="E51" s="32"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D52" s="31"/>
-      <c r="E52" s="32"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="29"/>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D53" s="31"/>
-      <c r="E53" s="32"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="29"/>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D54" s="31"/>
-      <c r="E54" s="32"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29"/>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D56" s="31"/>
-      <c r="E56" s="32"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="29"/>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D57" s="31"/>
-      <c r="E57" s="32"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="29"/>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D58" s="31"/>
-      <c r="E58" s="32"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="29"/>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D60" s="31"/>
-      <c r="E60" s="32"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="29"/>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="29"/>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D62" s="31"/>
-      <c r="E62" s="32"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="29"/>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="29"/>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D64" s="31"/>
-      <c r="E64" s="32"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="29"/>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D65" s="31"/>
-      <c r="E65" s="32"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="29"/>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D66" s="31"/>
-      <c r="E66" s="32"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="29"/>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D67" s="31"/>
-      <c r="E67" s="32"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="29"/>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D68" s="31"/>
-      <c r="E68" s="32"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="29"/>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D69" s="31"/>
-      <c r="E69" s="32"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="29"/>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="31"/>
-      <c r="E70" s="32"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="29"/>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D71" s="31"/>
-      <c r="E71" s="32"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="29"/>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D72" s="31"/>
-      <c r="E72" s="32"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="29"/>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D73" s="31"/>
-      <c r="E73" s="32"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="29"/>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D74" s="31"/>
-      <c r="E74" s="32"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="29"/>
     </row>
     <row r="75" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D75" s="31"/>
-      <c r="E75" s="32"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="29"/>
     </row>
     <row r="76" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D76" s="31"/>
-      <c r="E76" s="32"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="29"/>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D77" s="31"/>
-      <c r="E77" s="32"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="29"/>
     </row>
     <row r="78" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D78" s="31"/>
-      <c r="E78" s="32"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="29"/>
     </row>
     <row r="79" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D79" s="31"/>
-      <c r="E79" s="32"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="29"/>
     </row>
     <row r="80" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D80" s="31"/>
-      <c r="E80" s="32"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="29"/>
     </row>
     <row r="81" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D81" s="31"/>
-      <c r="E81" s="32"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="29"/>
     </row>
     <row r="82" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D82" s="31"/>
-      <c r="E82" s="32"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="29"/>
     </row>
     <row r="83" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D83" s="31"/>
-      <c r="E83" s="32"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="29"/>
     </row>
     <row r="84" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D84" s="31"/>
-      <c r="E84" s="32"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="29"/>
     </row>
     <row r="85" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D85" s="31"/>
-      <c r="E85" s="32"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="29"/>
     </row>
     <row r="86" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D86" s="31"/>
-      <c r="E86" s="32"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="29"/>
     </row>
     <row r="87" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D87" s="31"/>
-      <c r="E87" s="32"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="29"/>
     </row>
     <row r="88" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D88" s="31"/>
-      <c r="E88" s="32"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="29"/>
     </row>
     <row r="89" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D89" s="31"/>
-      <c r="E89" s="32"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="29"/>
     </row>
     <row r="90" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D90" s="31"/>
-      <c r="E90" s="32"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="29"/>
     </row>
     <row r="91" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D91" s="31"/>
-      <c r="E91" s="32"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="29"/>
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D92" s="31"/>
-      <c r="E92" s="32"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="29"/>
     </row>
     <row r="93" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D93" s="31"/>
-      <c r="E93" s="32"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="29"/>
     </row>
     <row r="94" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D94" s="31"/>
-      <c r="E94" s="32"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="29"/>
     </row>
     <row r="95" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D95" s="31"/>
-      <c r="E95" s="32"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="29"/>
     </row>
     <row r="96" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D96" s="31"/>
-      <c r="E96" s="32"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="29"/>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D97" s="31"/>
-      <c r="E97" s="32"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="29"/>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D98" s="31"/>
-      <c r="E98" s="32"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="29"/>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D99" s="31"/>
-      <c r="E99" s="32"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="29"/>
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D100" s="31"/>
-      <c r="E100" s="32"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="29"/>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D101" s="31"/>
-      <c r="E101" s="32"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="29"/>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D102" s="31"/>
-      <c r="E102" s="32"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="29"/>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D103" s="31"/>
-      <c r="E103" s="32"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="29"/>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D104" s="31"/>
-      <c r="E104" s="32"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="29"/>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D105" s="31"/>
-      <c r="E105" s="32"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="29"/>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D106" s="31"/>
-      <c r="E106" s="32"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="29"/>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D107" s="31"/>
-      <c r="E107" s="32"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="29"/>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D108" s="31"/>
-      <c r="E108" s="32"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="29"/>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D109" s="31"/>
-      <c r="E109" s="32"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="29"/>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D110" s="31"/>
-      <c r="E110" s="32"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="29"/>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D111" s="31"/>
-      <c r="E111" s="32"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="29"/>
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D112" s="31"/>
-      <c r="E112" s="32"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="29"/>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D113" s="31"/>
-      <c r="E113" s="32"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="29"/>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D114" s="31"/>
-      <c r="E114" s="32"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="29"/>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D115" s="31"/>
-      <c r="E115" s="32"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="29"/>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D116" s="31"/>
-      <c r="E116" s="32"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="29"/>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D117" s="31"/>
-      <c r="E117" s="32"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1875,26 +1928,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="125.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="37" customWidth="1"/>
+    <col min="2" max="3" width="25.85546875" style="37" customWidth="1"/>
+    <col min="4" max="4" width="125.28515625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="37" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1903,8 +1957,8 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
@@ -1912,19 +1966,19 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6"/>
@@ -1932,8 +1986,8 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6"/>
@@ -1941,8 +1995,8 @@
       <c r="D6" s="8"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="10"/>
@@ -1950,15 +2004,15 @@
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
@@ -1969,7 +2023,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="15"/>
@@ -1979,8 +2033,8 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="6"/>
@@ -1988,8 +2042,8 @@
       <c r="D11" s="16"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6"/>
@@ -1999,8 +2053,8 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6"/>
@@ -2008,8 +2062,8 @@
       <c r="D13" s="8"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10"/>
@@ -2027,17 +2081,17 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="42" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2045,16 +2099,16 @@
       <c r="A17" s="19">
         <v>1</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="45">
         <v>35</v>
       </c>
     </row>
@@ -2062,16 +2116,16 @@
       <c r="A18" s="19">
         <v>2</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2079,16 +2133,16 @@
       <c r="A19" s="19">
         <v>3</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2096,16 +2150,16 @@
       <c r="A20" s="19">
         <v>4</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="33">
         <v>45</v>
       </c>
     </row>
@@ -2113,16 +2167,16 @@
       <c r="A21" s="19">
         <v>5</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2130,16 +2184,16 @@
       <c r="A22" s="19">
         <v>6</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="33">
         <v>45</v>
       </c>
     </row>
@@ -2147,33 +2201,33 @@
       <c r="A23" s="19">
         <v>7</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="33">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>8</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="33">
         <v>30</v>
       </c>
     </row>
@@ -2181,16 +2235,16 @@
       <c r="A25" s="19">
         <v>9</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2198,16 +2252,16 @@
       <c r="A26" s="19">
         <v>10</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2215,16 +2269,16 @@
       <c r="A27" s="19">
         <v>11</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2232,16 +2286,16 @@
       <c r="A28" s="19">
         <v>12</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2249,50 +2303,50 @@
       <c r="A29" s="19">
         <v>13</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="33">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
         <v>14</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="33">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="19">
         <v>15</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2300,16 +2354,16 @@
       <c r="A32" s="19">
         <v>16</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="24">
+      <c r="E32" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2317,33 +2371,33 @@
       <c r="A33" s="19">
         <v>17</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="23" t="s">
+      <c r="D33" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="24">
+      <c r="E33" s="33">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="19">
         <v>18</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E34" s="33">
         <v>30</v>
       </c>
     </row>
@@ -2351,16 +2405,16 @@
       <c r="A35" s="19">
         <v>19</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="33">
         <v>45</v>
       </c>
     </row>
@@ -2368,16 +2422,16 @@
       <c r="A36" s="19">
         <v>20</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2385,16 +2439,16 @@
       <c r="A37" s="19">
         <v>21</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="33">
         <v>50</v>
       </c>
     </row>
@@ -2402,33 +2456,33 @@
       <c r="A38" s="19">
         <v>22</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="33">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
         <v>23</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="33">
         <v>40</v>
       </c>
     </row>
@@ -2436,33 +2490,33 @@
       <c r="A40" s="19">
         <v>24</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D40" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="33">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="19">
         <v>25</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="33">
         <v>30</v>
       </c>
     </row>
@@ -2471,5 +2525,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>